<commit_message>
iimproved aif selection by adding a screening for smoothness
</commit_message>
<xml_diff>
--- a/averaged_similarity_metrics_for_comparison.xlsx
+++ b/averaged_similarity_metrics_for_comparison.xlsx
@@ -477,10 +477,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.5103186941423578</v>
+        <v>0.8430004128481028</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5103186941423578</v>
+        <v>0.8430004128481028</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -501,10 +501,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.8161525210516997</v>
+        <v>0.8149991627413542</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8161525210516997</v>
+        <v>0.8149991627413542</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -525,10 +525,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2.949892710157555</v>
+        <v>0.983795667930816</v>
       </c>
       <c r="D4" t="n">
-        <v>2.949892710157555</v>
+        <v>0.983795667930816</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.6122074095865447</v>
+        <v>0.5283687264620415</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6122074095865447</v>
+        <v>0.5283687264620415</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -573,10 +573,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.717525170167109</v>
+        <v>0.9918647427602294</v>
       </c>
       <c r="D6" t="n">
-        <v>1.717525170167109</v>
+        <v>0.9918647427602294</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -597,10 +597,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5128191539243101</v>
+        <v>0.9552030896374605</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5128191539243101</v>
+        <v>0.9552030896374605</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.8280503686987305</v>
+        <v>0.8946756536048722</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8280503686987305</v>
+        <v>0.8946756536048722</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -645,10 +645,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.110681934757337</v>
+        <v>0.183381994295238</v>
       </c>
       <c r="D9" t="n">
-        <v>2.110681934757337</v>
+        <v>0.183381994295238</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -669,10 +669,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.435291979018326</v>
+        <v>0.1999529876236299</v>
       </c>
       <c r="D10" t="n">
-        <v>0.435291979018326</v>
+        <v>0.1999529876236299</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -693,10 +693,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.452818617294443</v>
+        <v>0.4282312392799456</v>
       </c>
       <c r="D11" t="n">
-        <v>1.452818617294443</v>
+        <v>0.4282312392799456</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -717,10 +717,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.5724127215705079</v>
+        <v>0.4251803619439751</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5724127215705079</v>
+        <v>0.4251803619439751</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -741,10 +741,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.7577632458178855</v>
+        <v>0.7413200363006528</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7577632458178855</v>
+        <v>0.7413200363006528</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -765,10 +765,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.4473196463448897</v>
+        <v>0.5718734448082547</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4473196463448897</v>
+        <v>0.5718734448082547</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.5168843946530898</v>
+        <v>0.5894519237919532</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5168843946530898</v>
+        <v>0.5894519237919532</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -813,10 +813,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.6688195917771023</v>
+        <v>0.7562231448509459</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6688195917771023</v>
+        <v>0.7562231448509459</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -837,10 +837,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.5402662576299544</v>
+        <v>0.6999368509667938</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5402662576299544</v>
+        <v>0.6999368509667938</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -861,10 +861,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.7798853339133838</v>
+        <v>0.8003200282938729</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7798853339133838</v>
+        <v>0.8003200282938729</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -885,10 +885,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.6000984586269685</v>
+        <v>0.69545189377858</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6000984586269685</v>
+        <v>0.69545189377858</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -909,10 +909,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.5775185447413985</v>
+        <v>0.5851580979618136</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5775185447413985</v>
+        <v>0.5851580979618136</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -933,10 +933,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.7746602214048225</v>
+        <v>0.8339375838625934</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7746602214048225</v>
+        <v>0.8339375838625934</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>

</xml_diff>